<commit_message>
updates label with Miscellanea. First not complete run
</commit_message>
<xml_diff>
--- a/output/dati.xlsx
+++ b/output/dati.xlsx
@@ -638,16 +638,16 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Residui: economia regionale, energia e ambiente, mercato immobiliare</t>
+          <t>Energia e ambiente, Economia regionale e mercato immobiliare</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Q, R, Y, Z, P, D9, A, B</t>
+          <t>Q, R</t>
         </is>
       </c>
       <c r="C11" t="n">
-        <v>0.049625468164794</v>
+        <v>0.04681647940074907</v>
       </c>
       <c r="D11" t="inlineStr">
         <is>
@@ -663,11 +663,11 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>D03, E01</t>
+          <t>E01, D03, P33</t>
         </is>
       </c>
       <c r="C12" t="n">
-        <v>0.007490636704119849</v>
+        <v>0.01029962546816479</v>
       </c>
       <c r="D12" t="inlineStr">
         <is>
@@ -858,16 +858,16 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Residui: economia regionale, energia e ambiente, mercato immobiliare</t>
+          <t>Energia e ambiente, Economia regionale e mercato immobiliare</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Q, R, Y, Z, P, D9, A, B</t>
+          <t>Q, R</t>
         </is>
       </c>
       <c r="C22" t="n">
-        <v>0.09770955165692008</v>
+        <v>0.05540935672514619</v>
       </c>
       <c r="D22" t="inlineStr">
         <is>
@@ -883,11 +883,11 @@
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>E71, E00</t>
+          <t>A2, B30, A23, Z1, B26, A1, B20, E00, D92, B17, B1, E71, Z31, Z3, Z10, B32, B31, B00, B27, P5, P16, D91, Z13</t>
         </is>
       </c>
       <c r="C23" t="n">
-        <v>0.001169590643274854</v>
+        <v>0.04346978557504873</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>

</xml_diff>